<commit_message>
worked with P10 to P11_..., made excel sheet with evaluations, P8 evaluation cannot be done because output not always in correct format
</commit_message>
<xml_diff>
--- a/data/evaluation_prompts.xlsx
+++ b/data/evaluation_prompts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shirin 1/git/PreclinicalAbstractClassification/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9F8EFDD-5531-1A45-BF53-18590806D497}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AC2D7EF-9635-3640-BF86-96D12CF65356}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="1000" windowWidth="25040" windowHeight="14400" xr2:uid="{8DEB04AB-2159-B140-83EF-22DC4E795892}"/>
+    <workbookView xWindow="2320" yWindow="1820" windowWidth="21380" windowHeight="14060" xr2:uid="{8DEB04AB-2159-B140-83EF-22DC4E795892}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="31">
   <si>
     <t>prompt description</t>
   </si>
@@ -108,13 +108,34 @@
   </si>
   <si>
     <t>summary gpt-4 test 50</t>
+  </si>
+  <si>
+    <t>P10</t>
+  </si>
+  <si>
+    <t>P11</t>
+  </si>
+  <si>
+    <t>P11_1</t>
+  </si>
+  <si>
+    <t>P11_2</t>
+  </si>
+  <si>
+    <t>P11_3</t>
+  </si>
+  <si>
+    <t>P11_4</t>
+  </si>
+  <si>
+    <t>summary gpt-4 1996 abstracts</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -129,13 +150,25 @@
       <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -150,12 +183,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -490,10 +526,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90BC467B-3818-CB45-90D9-07E8BC875ED8}">
-  <dimension ref="A1:K39"/>
+  <dimension ref="A1:K66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I23" sqref="I23:K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -504,20 +540,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="G1" s="2" t="s">
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="G1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -555,22 +591,67 @@
       <c r="A3" t="s">
         <v>5</v>
       </c>
+      <c r="C3">
+        <v>0.53082051282051201</v>
+      </c>
+      <c r="D3">
+        <v>0.36</v>
+      </c>
+      <c r="E3">
+        <v>0.34943196672608401</v>
+      </c>
       <c r="G3" t="s">
         <v>5</v>
+      </c>
+      <c r="I3" s="2">
+        <v>0.50564805999999995</v>
+      </c>
+      <c r="J3" s="2">
+        <v>0.25513784</v>
+      </c>
+      <c r="K3" s="2">
+        <v>0.20566124999999999</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>6</v>
       </c>
+      <c r="C4">
+        <v>0.61448717948717901</v>
+      </c>
+      <c r="D4">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="E4">
+        <v>0.28206060606060601</v>
+      </c>
       <c r="G4" t="s">
         <v>6</v>
+      </c>
+      <c r="I4" s="2">
+        <v>0.52365876</v>
+      </c>
+      <c r="J4" s="2">
+        <v>0.21804510999999999</v>
+      </c>
+      <c r="K4" s="2">
+        <v>0.16039635999999999</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>20</v>
       </c>
+      <c r="C5" s="2">
+        <v>0.19866666999999999</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0.24</v>
+      </c>
+      <c r="E5" s="2">
+        <v>0.20141176</v>
+      </c>
       <c r="G5" t="s">
         <v>20</v>
       </c>
@@ -579,6 +660,15 @@
       <c r="A6" t="s">
         <v>7</v>
       </c>
+      <c r="C6">
+        <v>0.3</v>
+      </c>
+      <c r="D6">
+        <v>0.06</v>
+      </c>
+      <c r="E6">
+        <v>9.9999999999999895E-2</v>
+      </c>
       <c r="G6" t="s">
         <v>7</v>
       </c>
@@ -587,6 +677,15 @@
       <c r="A7" t="s">
         <v>8</v>
       </c>
+      <c r="C7" s="2">
+        <v>0.55655677999999997</v>
+      </c>
+      <c r="D7" s="2">
+        <v>0.42</v>
+      </c>
+      <c r="E7" s="2">
+        <v>0.38225550000000003</v>
+      </c>
       <c r="G7" t="s">
         <v>8</v>
       </c>
@@ -595,6 +694,15 @@
       <c r="A8" t="s">
         <v>9</v>
       </c>
+      <c r="C8" s="2">
+        <v>0.54193650999999998</v>
+      </c>
+      <c r="D8" s="2">
+        <v>0.42</v>
+      </c>
+      <c r="E8" s="2">
+        <v>0.41297931999999998</v>
+      </c>
       <c r="G8" t="s">
         <v>9</v>
       </c>
@@ -603,6 +711,15 @@
       <c r="A9" t="s">
         <v>10</v>
       </c>
+      <c r="C9" s="2">
+        <v>0.56226496000000004</v>
+      </c>
+      <c r="D9" s="2">
+        <v>0.34</v>
+      </c>
+      <c r="E9" s="2">
+        <v>0.34794871999999999</v>
+      </c>
       <c r="G9" t="s">
         <v>10</v>
       </c>
@@ -611,6 +728,15 @@
       <c r="A10" t="s">
         <v>21</v>
       </c>
+      <c r="C10" s="2">
+        <v>0.54122221999999998</v>
+      </c>
+      <c r="D10" s="2">
+        <v>0.38</v>
+      </c>
+      <c r="E10" s="2">
+        <v>0.35797403</v>
+      </c>
       <c r="G10" t="s">
         <v>21</v>
       </c>
@@ -619,6 +745,15 @@
       <c r="A11" t="s">
         <v>11</v>
       </c>
+      <c r="C11">
+        <v>0.266666666666666</v>
+      </c>
+      <c r="D11">
+        <v>0.08</v>
+      </c>
+      <c r="E11">
+        <v>0.123076923076923</v>
+      </c>
       <c r="G11" t="s">
         <v>11</v>
       </c>
@@ -627,6 +762,15 @@
       <c r="A12" t="s">
         <v>12</v>
       </c>
+      <c r="C12" s="2">
+        <v>0.45187878999999997</v>
+      </c>
+      <c r="D12" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="E12" s="2">
+        <v>0.38677778000000002</v>
+      </c>
       <c r="G12" t="s">
         <v>12</v>
       </c>
@@ -643,153 +787,532 @@
       <c r="A14" t="s">
         <v>14</v>
       </c>
+      <c r="C14" s="2">
+        <v>0.60946153999999997</v>
+      </c>
+      <c r="D14" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="E14" s="2">
+        <v>0.47566386999999999</v>
+      </c>
       <c r="G14" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+      <c r="I14" s="2">
+        <v>0.61817975999999997</v>
+      </c>
+      <c r="J14" s="2">
+        <v>0.45162907000000002</v>
+      </c>
+      <c r="K14" s="2">
+        <v>0.44334500999999998</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="G15" t="s">
+      <c r="C15" s="5">
+        <v>0.71651947999999999</v>
+      </c>
+      <c r="D15" s="5">
+        <v>0.6</v>
+      </c>
+      <c r="E15" s="5">
+        <v>0.60289298999999996</v>
+      </c>
+      <c r="G15" s="4" t="s">
         <v>15</v>
+      </c>
+      <c r="I15" s="5">
+        <v>0.58481218000000001</v>
+      </c>
+      <c r="J15" s="5">
+        <v>0.50075188000000004</v>
+      </c>
+      <c r="K15" s="5">
+        <v>0.50386770999999997</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>16</v>
       </c>
+      <c r="C16">
+        <v>0.58333333333333304</v>
+      </c>
+      <c r="D16">
+        <v>0.34</v>
+      </c>
+      <c r="E16">
+        <v>0.34663015245623902</v>
+      </c>
       <c r="G16" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I16" s="2">
+        <v>0.47712673999999999</v>
+      </c>
+      <c r="J16" s="2">
+        <v>0.23208019999999999</v>
+      </c>
+      <c r="K16" s="2">
+        <v>0.17306158999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>17</v>
       </c>
+      <c r="C17">
+        <v>0.41599999999999998</v>
+      </c>
+      <c r="D17">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="E17">
+        <v>0.30499999999999899</v>
+      </c>
       <c r="G17" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>18</v>
       </c>
+      <c r="C18">
+        <v>0.58186813186813102</v>
+      </c>
+      <c r="D18">
+        <v>0.4</v>
+      </c>
+      <c r="E18">
+        <v>0.39490909090908999</v>
+      </c>
       <c r="G18" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A22" s="2" t="s">
+      <c r="I18" s="2">
+        <v>0.56425099999999995</v>
+      </c>
+      <c r="J18" s="2">
+        <v>0.27619048000000002</v>
+      </c>
+      <c r="K18" s="2">
+        <v>0.24500280999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19">
+        <v>0.655555555555555</v>
+      </c>
+      <c r="D19">
+        <v>0.38</v>
+      </c>
+      <c r="E19">
+        <v>0.40454545454545399</v>
+      </c>
+      <c r="G19" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20">
+        <v>0.60133333333333305</v>
+      </c>
+      <c r="D20">
+        <v>0.46</v>
+      </c>
+      <c r="E20">
+        <v>0.44543589743589701</v>
+      </c>
+      <c r="G20" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>26</v>
+      </c>
+      <c r="C21">
+        <v>0.54952380952380897</v>
+      </c>
+      <c r="D21">
+        <v>0.36</v>
+      </c>
+      <c r="E21">
+        <v>0.32374703557312201</v>
+      </c>
+      <c r="G21" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>27</v>
+      </c>
+      <c r="C22">
+        <v>0.47060606060605997</v>
+      </c>
+      <c r="D22">
+        <v>0.42</v>
+      </c>
+      <c r="E22">
+        <v>0.38861538461538397</v>
+      </c>
+      <c r="G22" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>28</v>
+      </c>
+      <c r="C23" s="2">
+        <v>0.69446154000000004</v>
+      </c>
+      <c r="D23" s="2">
+        <v>0.52</v>
+      </c>
+      <c r="E23" s="2">
+        <v>0.53914439000000003</v>
+      </c>
+      <c r="G23" t="s">
+        <v>28</v>
+      </c>
+      <c r="I23">
+        <v>0.60768</v>
+      </c>
+      <c r="J23">
+        <v>0.43959900000000002</v>
+      </c>
+      <c r="K23">
+        <v>0.435585</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>29</v>
+      </c>
+      <c r="C24" s="2">
+        <v>0.57015583999999997</v>
+      </c>
+      <c r="D24" s="2">
+        <v>0.54</v>
+      </c>
+      <c r="E24" s="2">
+        <v>0.51797541999999996</v>
+      </c>
+      <c r="G24" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A43" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A23" s="1" t="s">
+      <c r="B43" s="3"/>
+      <c r="C43" s="3"/>
+      <c r="D43" s="3"/>
+      <c r="E43" s="3"/>
+      <c r="G43" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="H43" s="3"/>
+      <c r="I43" s="3"/>
+      <c r="J43" s="3"/>
+      <c r="K43" s="3"/>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A44" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B44" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="C44" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="D44" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E23" s="1" t="s">
+      <c r="E44" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
+      <c r="G44" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H44" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I44" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J44" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K44" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
+      <c r="C45" s="2"/>
+      <c r="D45" s="2"/>
+      <c r="E45" s="2"/>
+      <c r="G45" t="s">
+        <v>5</v>
+      </c>
+      <c r="I45" s="2">
+        <v>0.59366505000000003</v>
+      </c>
+      <c r="J45" s="2">
+        <v>0.42506265999999998</v>
+      </c>
+      <c r="K45" s="2">
+        <v>0.40595713</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
+      <c r="C46" s="2"/>
+      <c r="D46" s="2"/>
+      <c r="E46" s="2"/>
+      <c r="G46" t="s">
+        <v>6</v>
+      </c>
+      <c r="I46" s="2">
+        <v>0.54637108999999995</v>
+      </c>
+      <c r="J46" s="2">
+        <v>0.36791980000000002</v>
+      </c>
+      <c r="K46" s="2">
+        <v>0.33070487999999998</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
+      <c r="G47" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
+      <c r="G48" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
+      <c r="C49" s="2">
+        <v>0.73085714000000002</v>
+      </c>
+      <c r="D49" s="2">
+        <v>0.64</v>
+      </c>
+      <c r="E49" s="2">
+        <v>0.66312265999999997</v>
+      </c>
+      <c r="G49" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
+      <c r="C50" s="2">
+        <v>0.72961905000000005</v>
+      </c>
+      <c r="D50" s="2">
+        <v>0.6</v>
+      </c>
+      <c r="E50" s="2">
+        <v>0.63242423999999997</v>
+      </c>
+      <c r="G50" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
+      <c r="C51" s="2">
+        <v>0.66476190000000002</v>
+      </c>
+      <c r="D51" s="2">
+        <v>0.38</v>
+      </c>
+      <c r="E51" s="2">
+        <v>0.46771021000000002</v>
+      </c>
+      <c r="G51" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
+      <c r="G52" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
+      <c r="G53" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
+      <c r="C54" s="2">
+        <v>0.77</v>
+      </c>
+      <c r="D54" s="2">
+        <v>0.68</v>
+      </c>
+      <c r="E54" s="2">
+        <v>0.70378644000000001</v>
+      </c>
+      <c r="G54" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
+      <c r="G55" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
+      <c r="G56" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
+      <c r="G57" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
+      <c r="G58" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
+      <c r="G59" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
         <v>18</v>
       </c>
+      <c r="B60" s="1"/>
+      <c r="C60" s="1"/>
+      <c r="D60" s="1"/>
+      <c r="E60" s="1"/>
+      <c r="G60" t="s">
+        <v>18</v>
+      </c>
+      <c r="H60" s="1"/>
+      <c r="I60" s="1"/>
+      <c r="J60" s="1"/>
+      <c r="K60" s="1"/>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>24</v>
+      </c>
+      <c r="G61" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>25</v>
+      </c>
+      <c r="G62" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>26</v>
+      </c>
+      <c r="G63" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>27</v>
+      </c>
+      <c r="G64" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>28</v>
+      </c>
+      <c r="G65" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>29</v>
+      </c>
+      <c r="G66" t="s">
+        <v>29</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="G1:K1"/>
-    <mergeCell ref="A22:E22"/>
+    <mergeCell ref="A43:E43"/>
+    <mergeCell ref="G43:K43"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
P11_1, P11_2, P11_4, P2_1
</commit_message>
<xml_diff>
--- a/data/evaluation_prompts.xlsx
+++ b/data/evaluation_prompts.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shirin 1/git/PreclinicalAbstractClassification/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AC2D7EF-9635-3640-BF86-96D12CF65356}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{468F678B-2C49-F14B-881E-AEC890C0E8CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2320" yWindow="1820" windowWidth="21380" windowHeight="14060" xr2:uid="{8DEB04AB-2159-B140-83EF-22DC4E795892}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="32">
   <si>
     <t>prompt description</t>
   </si>
@@ -129,13 +129,16 @@
   </si>
   <si>
     <t>summary gpt-4 1996 abstracts</t>
+  </si>
+  <si>
+    <t>&lt;=&gt; control classes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -156,8 +159,15 @@
       <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -167,6 +177,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -183,7 +199,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -192,6 +208,8 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -526,10 +544,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90BC467B-3818-CB45-90D9-07E8BC875ED8}">
-  <dimension ref="A1:K66"/>
+  <dimension ref="A1:L66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23:K23"/>
+      <selection activeCell="G24" activeCellId="1" sqref="G21:G22 G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -652,7 +670,7 @@
       <c r="E5" s="2">
         <v>0.20141176</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" s="7" t="s">
         <v>20</v>
       </c>
     </row>
@@ -689,6 +707,15 @@
       <c r="G7" t="s">
         <v>8</v>
       </c>
+      <c r="I7" s="2">
+        <v>0.57991552999999996</v>
+      </c>
+      <c r="J7" s="2">
+        <v>0.30175438999999998</v>
+      </c>
+      <c r="K7" s="2">
+        <v>0.27339846000000001</v>
+      </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
@@ -706,6 +733,15 @@
       <c r="G8" t="s">
         <v>9</v>
       </c>
+      <c r="I8" s="2">
+        <v>0.48737355999999998</v>
+      </c>
+      <c r="J8" s="2">
+        <v>0.31578947000000002</v>
+      </c>
+      <c r="K8" s="2">
+        <v>0.29975924999999998</v>
+      </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
@@ -723,6 +759,15 @@
       <c r="G9" t="s">
         <v>10</v>
       </c>
+      <c r="I9" s="2">
+        <v>0.48597420000000002</v>
+      </c>
+      <c r="J9" s="2">
+        <v>0.28671679</v>
+      </c>
+      <c r="K9" s="2">
+        <v>0.25912464000000002</v>
+      </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
@@ -740,6 +785,15 @@
       <c r="G10" t="s">
         <v>21</v>
       </c>
+      <c r="I10" s="2">
+        <v>0.51644239000000003</v>
+      </c>
+      <c r="J10" s="2">
+        <v>0.31528822000000001</v>
+      </c>
+      <c r="K10" s="2">
+        <v>0.30435465</v>
+      </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
@@ -774,6 +828,15 @@
       <c r="G12" t="s">
         <v>12</v>
       </c>
+      <c r="I12" s="2">
+        <v>0.55299197</v>
+      </c>
+      <c r="J12" s="2">
+        <v>0.36892230576441098</v>
+      </c>
+      <c r="K12" s="2">
+        <v>0.36742376660801201</v>
+      </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
@@ -782,6 +845,15 @@
       <c r="G13" t="s">
         <v>13</v>
       </c>
+      <c r="I13" s="2">
+        <v>0.53707185999999996</v>
+      </c>
+      <c r="J13" s="2">
+        <v>0.34486215999999997</v>
+      </c>
+      <c r="K13" s="2">
+        <v>0.33676861000000002</v>
+      </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
@@ -861,7 +933,7 @@
         <v>0.17306158999999999</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -878,7 +950,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -904,7 +976,7 @@
         <v>0.24500280999999999</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>24</v>
       </c>
@@ -920,8 +992,17 @@
       <c r="G19" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I19" s="2">
+        <v>0.51212380999999996</v>
+      </c>
+      <c r="J19" s="2">
+        <v>0.27669173000000002</v>
+      </c>
+      <c r="K19" s="2">
+        <v>0.24118174000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>25</v>
       </c>
@@ -937,8 +1018,17 @@
       <c r="G20" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I20" s="2">
+        <v>0.49125333999999998</v>
+      </c>
+      <c r="J20" s="2">
+        <v>0.30476189999999997</v>
+      </c>
+      <c r="K20" s="2">
+        <v>0.28231458999999998</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>26</v>
       </c>
@@ -951,11 +1041,11 @@
       <c r="E21">
         <v>0.32374703557312201</v>
       </c>
-      <c r="G21" t="s">
+      <c r="G21" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>27</v>
       </c>
@@ -968,11 +1058,11 @@
       <c r="E22">
         <v>0.38861538461538397</v>
       </c>
-      <c r="G22" t="s">
+      <c r="G22" s="7" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>28</v>
       </c>
@@ -997,8 +1087,11 @@
       <c r="K23">
         <v>0.435585</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L23" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>29</v>
       </c>
@@ -1011,7 +1104,7 @@
       <c r="E24" s="2">
         <v>0.51797541999999996</v>
       </c>
-      <c r="G24" t="s">
+      <c r="G24" s="7" t="s">
         <v>29</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Statistiken in Excel upgedatet von Evaluations of Prompts
</commit_message>
<xml_diff>
--- a/data/evaluation_prompts.xlsx
+++ b/data/evaluation_prompts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shirin 1/git/PreclinicalAbstractClassification/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{468F678B-2C49-F14B-881E-AEC890C0E8CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0480A9CC-04CF-A646-9E05-E7D7CBF7CFE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2320" yWindow="1820" windowWidth="21380" windowHeight="14060" xr2:uid="{8DEB04AB-2159-B140-83EF-22DC4E795892}"/>
   </bookViews>
@@ -167,7 +167,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -177,12 +177,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -199,7 +193,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -209,7 +203,8 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -546,8 +541,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90BC467B-3818-CB45-90D9-07E8BC875ED8}">
   <dimension ref="A1:L66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G24" activeCellId="1" sqref="G21:G22 G24"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -670,7 +665,7 @@
       <c r="E5" s="2">
         <v>0.20141176</v>
       </c>
-      <c r="G5" s="7" t="s">
+      <c r="G5" s="8" t="s">
         <v>20</v>
       </c>
     </row>
@@ -687,7 +682,7 @@
       <c r="E6">
         <v>9.9999999999999895E-2</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" s="6" t="s">
         <v>7</v>
       </c>
     </row>
@@ -808,7 +803,7 @@
       <c r="E11">
         <v>0.123076923076923</v>
       </c>
-      <c r="G11" t="s">
+      <c r="G11" s="6" t="s">
         <v>11</v>
       </c>
     </row>
@@ -946,7 +941,7 @@
       <c r="E17">
         <v>0.30499999999999899</v>
       </c>
-      <c r="G17" t="s">
+      <c r="G17" s="6" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1044,6 +1039,15 @@
       <c r="G21" s="7" t="s">
         <v>26</v>
       </c>
+      <c r="I21" s="2">
+        <v>0.48442905000000003</v>
+      </c>
+      <c r="J21" s="2">
+        <v>0.31578947000000002</v>
+      </c>
+      <c r="K21" s="2">
+        <v>0.29657749999999999</v>
+      </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
@@ -1061,6 +1065,15 @@
       <c r="G22" s="7" t="s">
         <v>27</v>
       </c>
+      <c r="I22" s="2">
+        <v>0.58530731000000003</v>
+      </c>
+      <c r="J22" s="2">
+        <v>0.32130325999999998</v>
+      </c>
+      <c r="K22" s="2">
+        <v>0.31364184000000001</v>
+      </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
@@ -1106,6 +1119,15 @@
       </c>
       <c r="G24" s="7" t="s">
         <v>29</v>
+      </c>
+      <c r="I24" s="2">
+        <v>0.58421833999999995</v>
+      </c>
+      <c r="J24" s="2">
+        <v>0.47518797000000002</v>
+      </c>
+      <c r="K24" s="2">
+        <v>0.48158585999999998</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
intermediate result excel-sheet evaluation_prompts
</commit_message>
<xml_diff>
--- a/data/evaluation_prompts.xlsx
+++ b/data/evaluation_prompts.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shirin 1/git/PreclinicalAbstractClassification/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0480A9CC-04CF-A646-9E05-E7D7CBF7CFE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EF077FB-3053-8647-B65C-791AA4BCCA6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2320" yWindow="1820" windowWidth="21380" windowHeight="14060" xr2:uid="{8DEB04AB-2159-B140-83EF-22DC4E795892}"/>
+    <workbookView xWindow="120" yWindow="500" windowWidth="21380" windowHeight="14060" xr2:uid="{8DEB04AB-2159-B140-83EF-22DC4E795892}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Evaluation_Summary" sheetId="3" r:id="rId1"/>
+    <sheet name="notes&amp;acronyms" sheetId="2" r:id="rId2"/>
+    <sheet name="other layout (incomplete)" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="67">
   <si>
     <t>prompt description</t>
   </si>
@@ -132,13 +134,188 @@
   </si>
   <si>
     <t>&lt;=&gt; control classes</t>
+  </si>
+  <si>
+    <t>CoT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CoT: Let's think step by step </t>
+  </si>
+  <si>
+    <t>CoT&amp;CC: based upon P11 (CoT placement with best results) but with original annotation guidelines, only table</t>
+  </si>
+  <si>
+    <t>CoT: step-by-step labeling. Doesn't work  yet because output format not always correct</t>
+  </si>
+  <si>
+    <t>notes</t>
+  </si>
+  <si>
+    <t>notes and acronyms</t>
+  </si>
+  <si>
+    <t>annotation guidelines: always without references</t>
+  </si>
+  <si>
+    <t>Chain-of-thought</t>
+  </si>
+  <si>
+    <t>CC</t>
+  </si>
+  <si>
+    <t>Contextual Clues</t>
+  </si>
+  <si>
+    <t>CC: original annotation guidelines, only table</t>
+  </si>
+  <si>
+    <t>CoT&amp;CC: shortened annotation guidelines &amp;Let's think step by step (CoT) put in different place than P11</t>
+  </si>
+  <si>
+    <t>CoT&amp;CC: shortened annotation guidelines &amp;Let's think step by step (CoT)</t>
+  </si>
+  <si>
+    <t>CoT&amp;CC: shortened annotation guidelines &amp;Let's think step by step (CoT) put in different place than P11 and P11_1</t>
+  </si>
+  <si>
+    <t>CC: original annotation guidelines</t>
+  </si>
+  <si>
+    <t>CoT&amp;CC: based upon P11 (CoT placement with best results) but with original annotation guidelines</t>
+  </si>
+  <si>
+    <t>"annotation guidelines" = table &amp; text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Px_y </t>
+  </si>
+  <si>
+    <t>Prompt x, further devloped, version y</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">CC: shortened annotation guidelines, only table </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow (Body)"/>
+      </rPr>
+      <t>didn't run on 1996 abstracts, because output on test50 wrong -&gt; bad evaluation</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">CC: shortened annotation guidelines, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow (Body)"/>
+      </rPr>
+      <t>didn't run on 1996 abstracts, because output on test50 wrong -&gt; bad evaluation</t>
+    </r>
+  </si>
+  <si>
+    <t>&lt;=&gt; control per class</t>
+  </si>
+  <si>
+    <t>CC: shortened annotation guidelines, only table; added separate mention of labels; reduced mentions of  what classification should apply to, format and where those infos occur</t>
+  </si>
+  <si>
+    <t>CC: shortened annotation guidelines, only table; based on P3_2, changed  wording: “list of annotations guidelines” to “following information for classification”</t>
+  </si>
+  <si>
+    <t>CC: shortened annotation guidelines,  based on P3_2 (better wording than P4 and most successful of P3-strategies)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">CC: shortened annotation guidelines,  based on P4_1 but “clinical study protocol” in guidelines instead of “study protocol” (P4_2), </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow (Body)"/>
+      </rPr>
+      <t>didn’t test on test50, because no protocol included in sample</t>
+    </r>
+  </si>
+  <si>
+    <t>CoT&amp;CC: short explanation why label was chosen + shortened annotation guidelines, only table</t>
+  </si>
+  <si>
+    <t>CoT: classification, short explanation why label was chosen</t>
+  </si>
+  <si>
+    <t>zero-shot: "Classify this text to one of these labels "</t>
+  </si>
+  <si>
+    <t>zero-shot: "Determine which of these labels fits the text best"</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">CC: shortened annotation guidelines, only table; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow (Body)"/>
+      </rPr>
+      <t>didn't run on 1996 abstracts, because output on test50 wrong, as didn't mention labels separately -&gt; bad results</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">zero-shot: added "The classfication applies to the journal name, title, and/or abstract of a study. " </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow (Body)"/>
+      </rPr>
+      <t>didn't run on 1996 abstracts, because output on test50 sometimes wrong</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">CoT: step-by-step labeling. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow (Body)"/>
+      </rPr>
+      <t>Doesn't work  yet because output format not always correct</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">didn't run on 1996 abstracts, because of </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow (Body)"/>
+      </rPr>
+      <t>what is written in red in the prompt description</t>
+    </r>
+  </si>
+  <si>
+    <t>example for significant performance differences on test50 vs. 1996 abstracts =&gt; Shirin will try to find a reason for this till the meeting</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -166,8 +343,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Aptos Narrow (Body)"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -180,8 +362,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.89999084444715716"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF9699"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -189,11 +389,39 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -205,12 +433,39 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF9699"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -538,18 +793,1023 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49E17E8F-075F-B54C-ACF4-C049684AF8E3}">
+  <dimension ref="B2:AA26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="67" workbookViewId="0">
+      <selection activeCell="K20" sqref="K20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="69" customWidth="1"/>
+    <col min="4" max="4" width="2.83203125" style="18" customWidth="1"/>
+    <col min="8" max="8" width="1.83203125" style="21" customWidth="1"/>
+    <col min="10" max="10" width="2.5" customWidth="1"/>
+    <col min="14" max="14" width="6.83203125" customWidth="1"/>
+    <col min="16" max="16" width="1.83203125" customWidth="1"/>
+    <col min="20" max="20" width="2" customWidth="1"/>
+    <col min="22" max="22" width="1.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="E2" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="10"/>
+      <c r="K2" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="L2" s="12"/>
+      <c r="M2" s="12"/>
+      <c r="N2" s="10"/>
+      <c r="O2" s="10"/>
+      <c r="Q2" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="R2" s="12"/>
+      <c r="S2" s="12"/>
+      <c r="T2" s="11"/>
+      <c r="U2" s="11"/>
+      <c r="W2" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="X2" s="12"/>
+      <c r="Y2" s="12"/>
+      <c r="Z2" s="10"/>
+      <c r="AA2" s="10"/>
+    </row>
+    <row r="3" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="B3" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H3" s="20"/>
+      <c r="I3" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="O3" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="T3" s="1"/>
+      <c r="U3" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="W3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="X3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="Y3" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="B4" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="E4">
+        <v>0.53082051282051201</v>
+      </c>
+      <c r="F4">
+        <v>0.36</v>
+      </c>
+      <c r="G4">
+        <v>0.34943196672608401</v>
+      </c>
+      <c r="I4" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="K4" s="2">
+        <v>0.50564805999999995</v>
+      </c>
+      <c r="L4" s="2">
+        <v>0.25513784</v>
+      </c>
+      <c r="M4" s="2">
+        <v>0.20566124999999999</v>
+      </c>
+      <c r="O4" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q4" s="2"/>
+      <c r="R4" s="2"/>
+      <c r="S4" s="2"/>
+      <c r="T4" s="2"/>
+      <c r="U4" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="W4" s="2">
+        <v>0.59366505000000003</v>
+      </c>
+      <c r="X4" s="2">
+        <v>0.42506265999999998</v>
+      </c>
+      <c r="Y4" s="2">
+        <v>0.40595713</v>
+      </c>
+    </row>
+    <row r="5" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="B5" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="E5">
+        <v>0.61448717948717901</v>
+      </c>
+      <c r="F5">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="G5">
+        <v>0.28206060606060601</v>
+      </c>
+      <c r="I5" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="K5" s="2">
+        <v>0.52365876</v>
+      </c>
+      <c r="L5" s="2">
+        <v>0.21804510999999999</v>
+      </c>
+      <c r="M5" s="2">
+        <v>0.16039635999999999</v>
+      </c>
+      <c r="O5" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q5" s="2"/>
+      <c r="R5" s="2"/>
+      <c r="S5" s="2"/>
+      <c r="T5" s="2"/>
+      <c r="U5" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="W5" s="2">
+        <v>0.54637108999999995</v>
+      </c>
+      <c r="X5" s="2">
+        <v>0.36791980000000002</v>
+      </c>
+      <c r="Y5" s="2">
+        <v>0.33070487999999998</v>
+      </c>
+    </row>
+    <row r="6" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="B6" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="E6" s="2">
+        <v>0.19866666999999999</v>
+      </c>
+      <c r="F6" s="2">
+        <v>0.24</v>
+      </c>
+      <c r="G6" s="2">
+        <v>0.20141176</v>
+      </c>
+      <c r="H6" s="22"/>
+      <c r="I6" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="K6" s="24"/>
+      <c r="L6" s="24"/>
+      <c r="M6" s="24"/>
+      <c r="O6" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="U6" s="15" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="B7" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="E7">
+        <v>0.3</v>
+      </c>
+      <c r="F7">
+        <v>0.06</v>
+      </c>
+      <c r="G7">
+        <v>9.9999999999999895E-2</v>
+      </c>
+      <c r="I7" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="K7" s="24"/>
+      <c r="L7" s="24"/>
+      <c r="M7" s="24"/>
+      <c r="O7" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="U7" s="15" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="B8" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="E8" s="2">
+        <v>0.55655677999999997</v>
+      </c>
+      <c r="F8" s="2">
+        <v>0.42</v>
+      </c>
+      <c r="G8" s="2">
+        <v>0.38225550000000003</v>
+      </c>
+      <c r="H8" s="22"/>
+      <c r="I8" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="K8" s="2">
+        <v>0.57991552999999996</v>
+      </c>
+      <c r="L8" s="2">
+        <v>0.30175438999999998</v>
+      </c>
+      <c r="M8" s="2">
+        <v>0.27339846000000001</v>
+      </c>
+      <c r="O8" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q8" s="2">
+        <v>0.73085714000000002</v>
+      </c>
+      <c r="R8" s="2">
+        <v>0.64</v>
+      </c>
+      <c r="S8" s="2">
+        <v>0.66312265999999997</v>
+      </c>
+      <c r="T8" s="2"/>
+      <c r="U8" s="14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="B9" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="E9" s="2">
+        <v>0.54193650999999998</v>
+      </c>
+      <c r="F9" s="2">
+        <v>0.42</v>
+      </c>
+      <c r="G9" s="2">
+        <v>0.41297931999999998</v>
+      </c>
+      <c r="H9" s="22"/>
+      <c r="I9" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="K9" s="2">
+        <v>0.48737355999999998</v>
+      </c>
+      <c r="L9" s="2">
+        <v>0.31578947000000002</v>
+      </c>
+      <c r="M9" s="2">
+        <v>0.29975924999999998</v>
+      </c>
+      <c r="O9" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q9" s="2">
+        <v>0.72961905000000005</v>
+      </c>
+      <c r="R9" s="2">
+        <v>0.6</v>
+      </c>
+      <c r="S9" s="2">
+        <v>0.63242423999999997</v>
+      </c>
+      <c r="T9" s="2"/>
+      <c r="U9" s="14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="B10" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="E10" s="2">
+        <v>0.56226496000000004</v>
+      </c>
+      <c r="F10" s="2">
+        <v>0.34</v>
+      </c>
+      <c r="G10" s="2">
+        <v>0.34794871999999999</v>
+      </c>
+      <c r="H10" s="22"/>
+      <c r="I10" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="K10" s="2">
+        <v>0.48597420000000002</v>
+      </c>
+      <c r="L10" s="2">
+        <v>0.28671679</v>
+      </c>
+      <c r="M10" s="2">
+        <v>0.25912464000000002</v>
+      </c>
+      <c r="O10" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q10" s="2">
+        <v>0.66476190000000002</v>
+      </c>
+      <c r="R10" s="2">
+        <v>0.38</v>
+      </c>
+      <c r="S10" s="2">
+        <v>0.46771021000000002</v>
+      </c>
+      <c r="T10" s="2"/>
+      <c r="U10" s="14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="B11" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="E11" s="2">
+        <v>0.54122221999999998</v>
+      </c>
+      <c r="F11" s="2">
+        <v>0.38</v>
+      </c>
+      <c r="G11" s="2">
+        <v>0.35797403</v>
+      </c>
+      <c r="H11" s="22"/>
+      <c r="I11" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="K11" s="2">
+        <v>0.51644239000000003</v>
+      </c>
+      <c r="L11" s="2">
+        <v>0.31528822000000001</v>
+      </c>
+      <c r="M11" s="2">
+        <v>0.30435465</v>
+      </c>
+      <c r="O11" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="U11" s="14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="B12" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="E12">
+        <v>0.266666666666666</v>
+      </c>
+      <c r="F12">
+        <v>0.08</v>
+      </c>
+      <c r="G12">
+        <v>0.123076923076923</v>
+      </c>
+      <c r="I12" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="K12" s="24"/>
+      <c r="L12" s="24"/>
+      <c r="M12" s="24"/>
+      <c r="O12" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="U12" s="15" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="B13" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="E13" s="2">
+        <v>0.45187878999999997</v>
+      </c>
+      <c r="F13" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="G13" s="2">
+        <v>0.38677778000000002</v>
+      </c>
+      <c r="H13" s="22"/>
+      <c r="I13" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="K13" s="2">
+        <v>0.55299197</v>
+      </c>
+      <c r="L13" s="2">
+        <v>0.36892230576441098</v>
+      </c>
+      <c r="M13" s="2">
+        <v>0.36742376660801201</v>
+      </c>
+      <c r="O13" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q13" s="2">
+        <v>0.77</v>
+      </c>
+      <c r="R13" s="2">
+        <v>0.68</v>
+      </c>
+      <c r="S13" s="2">
+        <v>0.70378644000000001</v>
+      </c>
+      <c r="T13" s="2"/>
+      <c r="U13" s="14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="B14" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="I14" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="K14" s="2">
+        <v>0.53707185999999996</v>
+      </c>
+      <c r="L14" s="2">
+        <v>0.34486215999999997</v>
+      </c>
+      <c r="M14" s="2">
+        <v>0.33676861000000002</v>
+      </c>
+      <c r="O14" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="U14" s="14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="B15" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="E15" s="2">
+        <v>0.60946153999999997</v>
+      </c>
+      <c r="F15" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="G15" s="2">
+        <v>0.47566386999999999</v>
+      </c>
+      <c r="H15" s="22"/>
+      <c r="I15" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="K15" s="2">
+        <v>0.61817975999999997</v>
+      </c>
+      <c r="L15" s="2">
+        <v>0.45162907000000002</v>
+      </c>
+      <c r="M15" s="2">
+        <v>0.44334500999999998</v>
+      </c>
+      <c r="O15" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="U15" s="14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="B16" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="E16" s="5">
+        <v>0.71651947999999999</v>
+      </c>
+      <c r="F16" s="5">
+        <v>0.6</v>
+      </c>
+      <c r="G16" s="5">
+        <v>0.60289298999999996</v>
+      </c>
+      <c r="H16" s="23"/>
+      <c r="I16" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="K16" s="5">
+        <v>0.58481218000000001</v>
+      </c>
+      <c r="L16" s="5">
+        <v>0.50075188000000004</v>
+      </c>
+      <c r="M16" s="5">
+        <v>0.50386770999999997</v>
+      </c>
+      <c r="O16" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="U16" s="14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B17" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="E17">
+        <v>0.58333333333333304</v>
+      </c>
+      <c r="F17">
+        <v>0.34</v>
+      </c>
+      <c r="G17">
+        <v>0.34663015245623902</v>
+      </c>
+      <c r="I17" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="K17" s="2">
+        <v>0.47712673999999999</v>
+      </c>
+      <c r="L17" s="2">
+        <v>0.23208019999999999</v>
+      </c>
+      <c r="M17" s="2">
+        <v>0.17306158999999999</v>
+      </c>
+      <c r="O17" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="U17" s="14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B18" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="E18">
+        <v>0.41599999999999998</v>
+      </c>
+      <c r="F18">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="G18">
+        <v>0.30499999999999899</v>
+      </c>
+      <c r="I18" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="K18" s="24"/>
+      <c r="L18" s="24"/>
+      <c r="M18" s="24"/>
+      <c r="O18" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="U18" s="15" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B19" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="E19">
+        <v>0.58186813186813102</v>
+      </c>
+      <c r="F19">
+        <v>0.4</v>
+      </c>
+      <c r="G19">
+        <v>0.39490909090908999</v>
+      </c>
+      <c r="I19" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="K19" s="2">
+        <v>0.56425099999999995</v>
+      </c>
+      <c r="L19" s="2">
+        <v>0.27619048000000002</v>
+      </c>
+      <c r="M19" s="2">
+        <v>0.24500280999999999</v>
+      </c>
+      <c r="O19" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="U19" s="14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B20" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="E20">
+        <v>0.655555555555555</v>
+      </c>
+      <c r="F20">
+        <v>0.38</v>
+      </c>
+      <c r="G20">
+        <v>0.40454545454545399</v>
+      </c>
+      <c r="I20" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="K20" s="2">
+        <v>0.51212380999999996</v>
+      </c>
+      <c r="L20" s="2">
+        <v>0.27669173000000002</v>
+      </c>
+      <c r="M20" s="2">
+        <v>0.24118174000000001</v>
+      </c>
+      <c r="O20" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="U20" s="14" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B21" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C21" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="E21">
+        <v>0.60133333333333305</v>
+      </c>
+      <c r="F21">
+        <v>0.46</v>
+      </c>
+      <c r="G21">
+        <v>0.44543589743589701</v>
+      </c>
+      <c r="I21" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="K21" s="2">
+        <v>0.49125333999999998</v>
+      </c>
+      <c r="L21" s="2">
+        <v>0.30476189999999997</v>
+      </c>
+      <c r="M21" s="2">
+        <v>0.28231458999999998</v>
+      </c>
+      <c r="O21" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="U21" s="14" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B22" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="C22" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="E22">
+        <v>0.54952380952380897</v>
+      </c>
+      <c r="F22">
+        <v>0.36</v>
+      </c>
+      <c r="G22">
+        <v>0.32374703557312201</v>
+      </c>
+      <c r="I22" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="K22" s="2">
+        <v>0.48442905000000003</v>
+      </c>
+      <c r="L22" s="2">
+        <v>0.31578947000000002</v>
+      </c>
+      <c r="M22" s="2">
+        <v>0.29657749999999999</v>
+      </c>
+      <c r="O22" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="U22" s="14" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B23" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C23" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="E23">
+        <v>0.47060606060605997</v>
+      </c>
+      <c r="F23">
+        <v>0.42</v>
+      </c>
+      <c r="G23">
+        <v>0.38861538461538397</v>
+      </c>
+      <c r="I23" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="K23" s="2">
+        <v>0.58530731000000003</v>
+      </c>
+      <c r="L23" s="2">
+        <v>0.32130325999999998</v>
+      </c>
+      <c r="M23" s="2">
+        <v>0.31364184000000001</v>
+      </c>
+      <c r="O23" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="U23" s="14" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="24" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B24" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="C24" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="E24" s="2">
+        <v>0.69446154000000004</v>
+      </c>
+      <c r="F24" s="2">
+        <v>0.52</v>
+      </c>
+      <c r="G24" s="2">
+        <v>0.53914439000000003</v>
+      </c>
+      <c r="H24" s="22"/>
+      <c r="I24" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="K24">
+        <v>0.60768</v>
+      </c>
+      <c r="L24">
+        <v>0.43959900000000002</v>
+      </c>
+      <c r="M24">
+        <v>0.435585</v>
+      </c>
+      <c r="N24" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="O24" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="U24" s="14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="25" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B25" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C25" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="E25" s="2">
+        <v>0.57015583999999997</v>
+      </c>
+      <c r="F25" s="2">
+        <v>0.54</v>
+      </c>
+      <c r="G25" s="2">
+        <v>0.51797541999999996</v>
+      </c>
+      <c r="H25" s="22"/>
+      <c r="I25" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="K25" s="2">
+        <v>0.58421833999999995</v>
+      </c>
+      <c r="L25" s="2">
+        <v>0.47518797000000002</v>
+      </c>
+      <c r="M25" s="2">
+        <v>0.48158585999999998</v>
+      </c>
+      <c r="O25" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="U25" s="14" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="26" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="C26" s="7"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="K2:M2"/>
+    <mergeCell ref="W2:Y2"/>
+    <mergeCell ref="Q2:S2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD7C6A26-482D-C04F-982C-E2185B2D0E99}">
+  <dimension ref="A1:B11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="24"/>
+      <c r="B6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="4"/>
+      <c r="B7" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>49</v>
+      </c>
+      <c r="B9" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B11" t="s">
+        <v>41</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:XFD1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90BC467B-3818-CB45-90D9-07E8BC875ED8}">
   <dimension ref="A1:L66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView zoomScale="41" workbookViewId="0">
+      <selection activeCell="A43" sqref="A43:E43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.33203125" customWidth="1"/>
     <col min="2" max="2" width="33.1640625" customWidth="1"/>
-    <col min="8" max="8" width="23.1640625" customWidth="1"/>
+    <col min="8" max="8" width="68.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
@@ -685,6 +1945,9 @@
       <c r="G6" s="6" t="s">
         <v>7</v>
       </c>
+      <c r="H6" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
@@ -806,6 +2069,9 @@
       <c r="G11" s="6" t="s">
         <v>11</v>
       </c>
+      <c r="H11" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
@@ -866,6 +2132,9 @@
       <c r="G14" t="s">
         <v>14</v>
       </c>
+      <c r="H14" t="s">
+        <v>42</v>
+      </c>
       <c r="I14" s="2">
         <v>0.61817975999999997</v>
       </c>
@@ -892,6 +2161,9 @@
       <c r="G15" s="4" t="s">
         <v>15</v>
       </c>
+      <c r="H15" s="4" t="s">
+        <v>46</v>
+      </c>
       <c r="I15" s="5">
         <v>0.58481218000000001</v>
       </c>
@@ -944,6 +2216,9 @@
       <c r="G17" s="6" t="s">
         <v>17</v>
       </c>
+      <c r="H17" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
@@ -987,6 +2262,9 @@
       <c r="G19" t="s">
         <v>24</v>
       </c>
+      <c r="H19" t="s">
+        <v>33</v>
+      </c>
       <c r="I19" s="2">
         <v>0.51212380999999996</v>
       </c>
@@ -1013,6 +2291,9 @@
       <c r="G20" t="s">
         <v>25</v>
       </c>
+      <c r="H20" t="s">
+        <v>44</v>
+      </c>
       <c r="I20" s="2">
         <v>0.49125333999999998</v>
       </c>
@@ -1039,6 +2320,9 @@
       <c r="G21" s="7" t="s">
         <v>26</v>
       </c>
+      <c r="H21" t="s">
+        <v>43</v>
+      </c>
       <c r="I21" s="2">
         <v>0.48442905000000003</v>
       </c>
@@ -1065,6 +2349,9 @@
       <c r="G22" s="7" t="s">
         <v>27</v>
       </c>
+      <c r="H22" t="s">
+        <v>45</v>
+      </c>
       <c r="I22" s="2">
         <v>0.58530731000000003</v>
       </c>
@@ -1091,6 +2378,9 @@
       <c r="G23" t="s">
         <v>28</v>
       </c>
+      <c r="H23" t="s">
+        <v>34</v>
+      </c>
       <c r="I23">
         <v>0.60768</v>
       </c>
@@ -1120,6 +2410,9 @@
       <c r="G24" s="7" t="s">
         <v>29</v>
       </c>
+      <c r="H24" t="s">
+        <v>47</v>
+      </c>
       <c r="I24" s="2">
         <v>0.58421833999999995</v>
       </c>
@@ -1128,6 +2421,11 @@
       </c>
       <c r="K24" s="2">
         <v>0.48158585999999998</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.2">

</xml_diff>